<commit_message>
Add Ver componente creado
</commit_message>
<xml_diff>
--- a/src/Data/colores.xlsx
+++ b/src/Data/colores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dsmith\Documents\Tesis\moduloprueba\src\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\Tesis\ModuloPersonalizable\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1220,16 +1220,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="J199" sqref="J199"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>50</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>'#ffebee',</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>'#ffcdd2',</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>200</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>'#ef9a9a',</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>300</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>'#e57373',</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>400</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>'#ef5350',</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>500</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>'#f44336',</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>600</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>'#e53935',</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>700</v>
       </c>
@@ -1373,7 +1372,7 @@
         <v>'#d32f2f',</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>800</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>'#c62828',</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>900</v>
       </c>
@@ -1409,7 +1408,7 @@
         <v>'#b71c1c',</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>'#ff8a80',</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>'#ff5252',</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>'#ff1744',</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>'#d50000',</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>50</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>'#fce4ec',</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>'#f8bbd0',</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>200</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>'#f48fb1',</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>300</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>'#f06292',</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>400</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>'#ec407a',</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>500</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>'#e91e63',</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>600</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>'#d81b60',</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>700</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>'#c2185b',</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>800</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>'#ad1457',</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>900</v>
       </c>
@@ -1661,7 +1660,7 @@
         <v>'#880e4f',</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>'#ff80ab',</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>'#ff4081',</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>'#f50057',</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>'#c51162',</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>50</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>'#f3e5f5',</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>100</v>
       </c>
@@ -1769,7 +1768,7 @@
         <v>'#e1bee7',</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>200</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>'#ce93d8',</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>300</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>'#ba68c8',</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>400</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>'#ab47bc',</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>500</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>'#9c27b0',</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>600</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>'#8e24aa',</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>700</v>
       </c>
@@ -1877,7 +1876,7 @@
         <v>'#7b1fa2',</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>800</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>'#6a1b9a',</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>900</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>'#4a148c',</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>'#ea80fc',</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>'#e040fb',</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>'#d500f9',</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>'#aa00ff',</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>50</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>'#ede7f6',</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>100</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>'#d1c4e9',</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>200</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>'#b39ddb',</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>300</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>'#9575cd',</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>400</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>'#7e57c2',</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>500</v>
       </c>
@@ -2093,7 +2092,7 @@
         <v>'#673ab7',</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>600</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>'#5e35b1',</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>700</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>'#512da8',</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>800</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>'#4527a0',</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>900</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>'#311b92',</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>'#b388ff',</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>'#7c4dff',</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>'#651fff',</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>35</v>
       </c>
@@ -2237,7 +2236,7 @@
         <v>'#6200ea',</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>50</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>'#e8eaf6',</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>100</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>'#c5cae9',</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>200</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>'#9fa8da',</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>300</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>'#7986cb',</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>400</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>'#5c6bc0',</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>500</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>'#3f51b5',</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>600</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>'#3949ab',</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>700</v>
       </c>
@@ -2381,7 +2380,7 @@
         <v>'#303f9f',</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>800</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>'#283593',</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>900</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>'#1a237e',</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -2435,7 +2434,7 @@
         <v>'#8c9eff',</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>'#536dfe',</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>33</v>
       </c>
@@ -2471,7 +2470,7 @@
         <v>'#3d5afe',</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -2489,7 +2488,7 @@
         <v>'#304ffe',</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>50</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>'#e3f2fd',</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>100</v>
       </c>
@@ -2525,7 +2524,7 @@
         <v>'#bbdefb',</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>200</v>
       </c>
@@ -2543,7 +2542,7 @@
         <v>'#90caf9',</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>300</v>
       </c>
@@ -2561,7 +2560,7 @@
         <v>'#64b5f6',</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>400</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>'#42a5f5',</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>500</v>
       </c>
@@ -2597,7 +2596,7 @@
         <v>'#2196f3',</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>600</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>'#1e88e5',</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>700</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>'#1976d2',</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>800</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>'#1565c0',</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>900</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>'#0d47a1',</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -2687,7 +2686,7 @@
         <v>'#82b1ff',</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>31</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>'#448aff',</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>'#2979ff',</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>35</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>'#2962ff',</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>50</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>'#e1f5fe',</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>100</v>
       </c>
@@ -2777,7 +2776,7 @@
         <v>'#b3e5fc',</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>200</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>'#81d4fa',</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>300</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>'#4fc3f7',</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>400</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>'#29b6f6',</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>500</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>'#03a9f4',</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>600</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>'#039be5',</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>700</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>'#0288d1',</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>800</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>'#0277bd',</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>900</v>
       </c>
@@ -2921,7 +2920,7 @@
         <v>'#01579b',</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>'#80d8ff',</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>'#40c4ff',</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>33</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>'#00b0ff',</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>35</v>
       </c>
@@ -2993,7 +2992,7 @@
         <v>'#0091ea',</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>50</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>'#e0f7fa',</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>100</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>'#b2ebf2',</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>200</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>'#80deea',</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>300</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v>'#4dd0e1',</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>400</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>'#26c6da',</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>500</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>'#00bcd4',</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>600</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>'#00acc1',</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>700</v>
       </c>
@@ -3138,7 +3137,7 @@
         <v>'#0097a7',</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>800</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>'#00838f',</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>900</v>
       </c>
@@ -3174,7 +3173,7 @@
         <v>'#006064',</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>29</v>
       </c>
@@ -3192,7 +3191,7 @@
         <v>'#84ffff',</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>'#18ffff',</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>'#00e5ff',</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>35</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>'#00b8d4',</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>50</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>'#e0f2f1',</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>100</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>'#b2dfdb',</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>200</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>'#80cbc4',</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>300</v>
       </c>
@@ -3318,7 +3317,7 @@
         <v>'#4db6ac',</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>400</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>'#26a69a',</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>500</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>'#009688',</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>600</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>'#00897b',</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>700</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>'#00796b',</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>800</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>'#00695c',</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>900</v>
       </c>
@@ -3426,7 +3425,7 @@
         <v>'#004d40',</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>29</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>'#a7ffeb',</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>31</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>'#64ffda',</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>33</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>'#1de9b6',</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>35</v>
       </c>
@@ -3498,7 +3497,7 @@
         <v>'#00bfa5',</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>50</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>'#e8f5e9',</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>100</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>'#c8e6c9',</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>200</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>'#a5d6a7',</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>300</v>
       </c>
@@ -3570,7 +3569,7 @@
         <v>'#81c784',</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>400</v>
       </c>
@@ -3588,7 +3587,7 @@
         <v>'#66bb6a',</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>500</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>'#4caf50',</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>600</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>'#43a047',</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>700</v>
       </c>
@@ -3642,7 +3641,7 @@
         <v>'#388e3c',</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>800</v>
       </c>
@@ -3660,7 +3659,7 @@
         <v>'#2e7d32',</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>900</v>
       </c>
@@ -3678,7 +3677,7 @@
         <v>'#1b5e20',</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>29</v>
       </c>
@@ -3696,7 +3695,7 @@
         <v>'#b9f6ca',</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>31</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>'#69f0ae',</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>33</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>'#00e676',</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>'#00c853',</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>50</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>'#f1f8e9',</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>100</v>
       </c>
@@ -3786,7 +3785,7 @@
         <v>'#dcedc8',</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>200</v>
       </c>
@@ -3804,7 +3803,7 @@
         <v>'#c5e1a5',</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>300</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>'#aed581',</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>400</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>'#9ccc65',</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>500</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>'#8bc34a',</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>600</v>
       </c>
@@ -3876,7 +3875,7 @@
         <v>'#7cb342',</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>700</v>
       </c>
@@ -3894,7 +3893,7 @@
         <v>'#689f38',</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>800</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>'#558b2f',</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>900</v>
       </c>
@@ -3930,7 +3929,7 @@
         <v>'#33691e',</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>29</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>'#ccff90',</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>31</v>
       </c>
@@ -3966,7 +3965,7 @@
         <v>'#b2ff59',</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>33</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>'#76ff03',</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>35</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>'#64dd17',</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>50</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>'#f9fbe7',</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>100</v>
       </c>
@@ -4038,7 +4037,7 @@
         <v>'#f0f4c3',</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>200</v>
       </c>
@@ -4056,7 +4055,7 @@
         <v>'#e6ee9c',</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>300</v>
       </c>
@@ -4074,7 +4073,7 @@
         <v>'#dce775',</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>400</v>
       </c>
@@ -4092,7 +4091,7 @@
         <v>'#d4e157',</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>500</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>'#cddc39',</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>600</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>'#c0ca33',</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>700</v>
       </c>
@@ -4146,7 +4145,7 @@
         <v>'#afb42b',</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>800</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>'#9e9d24',</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>900</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>'#827717',</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>29</v>
       </c>
@@ -4200,7 +4199,7 @@
         <v>'#f4ff81',</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>31</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>'#eeff41',</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>33</v>
       </c>
@@ -4236,7 +4235,7 @@
         <v>'#c6ff00',</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -4254,7 +4253,7 @@
         <v>'#aeea00',</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>50</v>
       </c>
@@ -4272,7 +4271,7 @@
         <v>'#fffde7',</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>100</v>
       </c>
@@ -4290,7 +4289,7 @@
         <v>'#fff9c4',</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>200</v>
       </c>
@@ -4308,7 +4307,7 @@
         <v>'#fff59d',</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>300</v>
       </c>
@@ -4326,7 +4325,7 @@
         <v>'#fff176',</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>400</v>
       </c>
@@ -4344,7 +4343,7 @@
         <v>'#ffee58',</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>500</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>'#ffeb3b',</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>600</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>'#fdd835',</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>700</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>'#fbc02d',</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>800</v>
       </c>
@@ -4416,7 +4415,7 @@
         <v>'#f9a825',</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>900</v>
       </c>
@@ -4434,7 +4433,7 @@
         <v>'#f57f17',</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>29</v>
       </c>
@@ -4452,7 +4451,7 @@
         <v>'#ffff8d',</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>31</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>'#ffff00',</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>33</v>
       </c>
@@ -4488,7 +4487,7 @@
         <v>'#ffea00',</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -4506,7 +4505,7 @@
         <v>'#ffd600',</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>50</v>
       </c>
@@ -4524,7 +4523,7 @@
         <v>'#fff8e1',</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>100</v>
       </c>
@@ -4542,7 +4541,7 @@
         <v>'#ffecb3',</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>200</v>
       </c>
@@ -4560,7 +4559,7 @@
         <v>'#ffe082',</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>300</v>
       </c>
@@ -4578,7 +4577,7 @@
         <v>'#ffd54f',</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>400</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>'#ffca28',</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>500</v>
       </c>
@@ -4614,7 +4613,7 @@
         <v>'#ffc107',</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>600</v>
       </c>
@@ -4632,7 +4631,7 @@
         <v>'#ffb300',</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>700</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>'#ffa000',</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>800</v>
       </c>
@@ -4668,7 +4667,7 @@
         <v>'#ff8f00',</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>900</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>'#ff6f00',</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>29</v>
       </c>
@@ -4704,7 +4703,7 @@
         <v>'#ffe57f',</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>31</v>
       </c>
@@ -4722,7 +4721,7 @@
         <v>'#ffd740',</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>33</v>
       </c>
@@ -4740,7 +4739,7 @@
         <v>'#ffc400',</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>35</v>
       </c>
@@ -4758,7 +4757,7 @@
         <v>'#ffab00',</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>50</v>
       </c>
@@ -4776,7 +4775,7 @@
         <v>'#fff3e0',</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>100</v>
       </c>
@@ -4794,7 +4793,7 @@
         <v>'#ffe0b2',</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>200</v>
       </c>
@@ -4812,7 +4811,7 @@
         <v>'#ffcc80',</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>300</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>'#ffb74d',</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>400</v>
       </c>
@@ -4848,7 +4847,7 @@
         <v>'#ffa726',</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>500</v>
       </c>
@@ -4866,7 +4865,7 @@
         <v>'#ff9800',</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>600</v>
       </c>
@@ -4884,7 +4883,7 @@
         <v>'#fb8c00',</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>700</v>
       </c>
@@ -4902,7 +4901,7 @@
         <v>'#f57c00',</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>800</v>
       </c>
@@ -4920,7 +4919,7 @@
         <v>'#ef6c00',</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>900</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>'#e65100',</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>29</v>
       </c>
@@ -4956,7 +4955,7 @@
         <v>'#ffd180',</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>31</v>
       </c>
@@ -4974,7 +4973,7 @@
         <v>'#ffab40',</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>33</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>'#ff9100',</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>35</v>
       </c>
@@ -5010,7 +5009,7 @@
         <v>'#ff6d00',</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>50</v>
       </c>
@@ -5028,7 +5027,7 @@
         <v>'#fbe9e7',</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>100</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>'#ffccbc',</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>200</v>
       </c>
@@ -5064,7 +5063,7 @@
         <v>'#ffab91',</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>300</v>
       </c>
@@ -5082,7 +5081,7 @@
         <v>'#ff8a65',</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>400</v>
       </c>
@@ -5100,7 +5099,7 @@
         <v>'#ff7043',</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>500</v>
       </c>
@@ -5118,7 +5117,7 @@
         <v>'#ff5722',</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>600</v>
       </c>
@@ -5136,7 +5135,7 @@
         <v>'#f4511e',</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>700</v>
       </c>
@@ -5154,7 +5153,7 @@
         <v>'#e64a19',</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>800</v>
       </c>
@@ -5172,7 +5171,7 @@
         <v>'#d84315',</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>900</v>
       </c>
@@ -5190,7 +5189,7 @@
         <v>'#bf360c',</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>29</v>
       </c>
@@ -5208,7 +5207,7 @@
         <v>'#ff9e80',</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>31</v>
       </c>
@@ -5226,7 +5225,7 @@
         <v>'#ff6e40',</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>33</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>'#ff3d00',</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>35</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>'#dd2c00',</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>50</v>
       </c>
@@ -5280,7 +5279,7 @@
         <v>'#efebe9',</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>100</v>
       </c>
@@ -5298,7 +5297,7 @@
         <v>'#d7ccc8',</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>200</v>
       </c>
@@ -5316,7 +5315,7 @@
         <v>'#bcaaa4',</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>300</v>
       </c>
@@ -5334,7 +5333,7 @@
         <v>'#a1887f',</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>400</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>'#8d6e63',</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>500</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>'#795548',</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>600</v>
       </c>
@@ -5388,7 +5387,7 @@
         <v>'#6d4c41',</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>700</v>
       </c>
@@ -5406,7 +5405,7 @@
         <v>'#5d4037',</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>800</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>'#4e342e',</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>900</v>
       </c>
@@ -5442,7 +5441,7 @@
         <v>'#3e2723',</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>50</v>
       </c>
@@ -5460,7 +5459,7 @@
         <v>'#fafafa',</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>100</v>
       </c>
@@ -5478,7 +5477,7 @@
         <v>'#f5f5f5',</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>200</v>
       </c>
@@ -5496,7 +5495,7 @@
         <v>'#eeeeee',</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>300</v>
       </c>
@@ -5514,7 +5513,7 @@
         <v>'#e0e0e0',</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>400</v>
       </c>
@@ -5532,7 +5531,7 @@
         <v>'#bdbdbd',</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>500</v>
       </c>
@@ -5550,7 +5549,7 @@
         <v>'#9e9e9e',</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>600</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>'#757575',</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>700</v>
       </c>
@@ -5586,7 +5585,7 @@
         <v>'#616161',</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>800</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>'#424242',</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>900</v>
       </c>
@@ -5622,7 +5621,7 @@
         <v>'#212121',</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>50</v>
       </c>
@@ -5640,7 +5639,7 @@
         <v>'#eceff1',</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>100</v>
       </c>
@@ -5658,7 +5657,7 @@
         <v>'#cfd8dc',</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>200</v>
       </c>
@@ -5676,7 +5675,7 @@
         <v>'#b0bec5',</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>300</v>
       </c>
@@ -5694,7 +5693,7 @@
         <v>'#90a4ae',</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>400</v>
       </c>
@@ -5712,7 +5711,7 @@
         <v>'#78909c',</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>500</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>'#607d8b',</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>600</v>
       </c>
@@ -5748,7 +5747,7 @@
         <v>'#546e7a',</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>700</v>
       </c>
@@ -5766,7 +5765,7 @@
         <v>'#455a64',</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>800</v>
       </c>
@@ -5784,7 +5783,7 @@
         <v>'#37474f',</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>900</v>
       </c>
@@ -5803,22 +5802,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A254">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="100"/>
-        <filter val="200"/>
-        <filter val="300"/>
-        <filter val="400"/>
-        <filter val="50"/>
-        <filter val="500"/>
-        <filter val="600"/>
-        <filter val="700"/>
-        <filter val="800"/>
-        <filter val="900"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>